<commit_message>
Pooled Seesion Timed Out TCs
</commit_message>
<xml_diff>
--- a/Demo/SFS_SmokeTest/TestCases_Docs/ATX_P0testcases.xlsx
+++ b/Demo/SFS_SmokeTest/TestCases_Docs/ATX_P0testcases.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation Framework\new prog\ATX\wk.automation.suite.ATX\ClassLibrary1\SFS_SmokeTest\TestCases_Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation Framework SFS\New Project_SFS\wk.support.sfs.ATX_QA\Demo\SFS_SmokeTest\TestCases_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FB1061-9B40-4B3C-88D0-356C0F3588AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{860C6F46-9518-42DE-B27C-88CE1946620D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B389FAE1-FDED-4610-8300-114D2B489EFF}"/>
   </bookViews>
   <sheets>
-    <sheet name="ATX_Homepage" sheetId="1" r:id="rId1"/>
-    <sheet name="ATX_Menupage" sheetId="3" r:id="rId2"/>
+    <sheet name="P0_TC_ATX_Homepage" sheetId="1" r:id="rId1"/>
+    <sheet name="P1_TC" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="162">
   <si>
     <t>Sr no</t>
   </si>
@@ -1010,8 +1010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A9A0EA-E752-4DB4-8070-4BB8A6A50C23}">
   <dimension ref="A1:L162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G22" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="H30" zoomScale="65" zoomScaleNormal="102" workbookViewId="0">
+      <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1134,9 +1134,15 @@
       <c r="H4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
+      <c r="I4" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>29</v>
+      </c>
       <c r="L4" s="8"/>
     </row>
     <row r="5" spans="1:12" s="7" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
@@ -1164,9 +1170,15 @@
       <c r="H5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
+      <c r="I5" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>29</v>
+      </c>
       <c r="L5" s="8"/>
     </row>
     <row r="6" spans="1:12" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.3">
@@ -2113,9 +2125,15 @@
       <c r="H39" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8"/>
-      <c r="K39" s="8"/>
+      <c r="I39" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="J39" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K39" s="9" t="s">
+        <v>29</v>
+      </c>
       <c r="L39" s="8"/>
     </row>
     <row r="40" spans="1:12" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -2141,12 +2159,18 @@
       <c r="H40" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="I40" s="8"/>
-      <c r="J40" s="8"/>
-      <c r="K40" s="8"/>
+      <c r="I40" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="J40" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K40" s="9" t="s">
+        <v>29</v>
+      </c>
       <c r="L40" s="8"/>
     </row>
-    <row r="41" spans="1:12" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="s">
         <v>137</v>
       </c>
@@ -2169,12 +2193,18 @@
       <c r="H41" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="I41" s="8"/>
-      <c r="J41" s="8"/>
-      <c r="K41" s="8"/>
+      <c r="I41" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="J41" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K41" s="9" t="s">
+        <v>29</v>
+      </c>
       <c r="L41" s="8"/>
     </row>
-    <row r="42" spans="1:12" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A42" s="8" t="s">
         <v>138</v>
       </c>
@@ -2197,12 +2227,18 @@
       <c r="H42" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="I42" s="8"/>
-      <c r="J42" s="8"/>
-      <c r="K42" s="8"/>
+      <c r="I42" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="J42" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K42" s="9" t="s">
+        <v>29</v>
+      </c>
       <c r="L42" s="8"/>
     </row>
-    <row r="43" spans="1:12" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A43" s="8" t="s">
         <v>139</v>
       </c>
@@ -2225,9 +2261,15 @@
       <c r="H43" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="I43" s="8"/>
-      <c r="J43" s="8"/>
-      <c r="K43" s="8"/>
+      <c r="I43" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="J43" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K43" s="9" t="s">
+        <v>29</v>
+      </c>
       <c r="L43" s="8"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
@@ -3678,8 +3720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A014A9DB-ACD2-44BB-9B56-46AA4F450CAE}">
   <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>